<commit_message>
Adds Rules to DPV, fixes typos in IRIs
- see #284 (was Use-Cases)
- Adds new Rules to DPV: Recommendation, Deterrence
- Contains updated RDF and HTML outputs
- Fixes typo in IRI of hasFulfilmentStatus (breaking change)

Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
Co-authored-by: Georg P. Krog <georg@signatu.com>
Co-authored-by: Paul Ryan <71695536+Paul-Ryan76@users.noreply.github.com>
Co-authored-by: Julian Flake <flake@uni-koblenz.de>
Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/rules.xlsx
+++ b/code/vocab_csv/rules.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="134">
   <si>
     <t>Term</t>
   </si>
@@ -77,13 +77,79 @@
     <t>Harshvardhan J. Pandit, Georg P. Krog, Beatriz Esteves, Paul Ryan</t>
   </si>
   <si>
+    <t>AcceptableRule</t>
+  </si>
+  <si>
+    <t>Acceptable Rule</t>
+  </si>
+  <si>
+    <t>A rule that is acceptable where it is either desirable if it occurs or it is not unacceptable if it does</t>
+  </si>
+  <si>
+    <t>dpv:Rule</t>
+  </si>
+  <si>
+    <t>Acceptable is a subjective concept that enables distinguishing with "unacceptable". By itself it does not signal any permission or obligation - for which further specific concepts are defined</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Delaram Golpayegani, Beatriz Esteves, Arthit Suriyawongkul, Paul Ryan</t>
+  </si>
+  <si>
     <t>Permission</t>
   </si>
   <si>
     <t>A rule describing a permission to perform an activity</t>
   </si>
   <si>
-    <t>dpv:Rule</t>
+    <t>dpv:AcceptableRule</t>
+  </si>
+  <si>
+    <t>Permissions are aligned with the term MAY in RFC2119 where specified activities may or may not be carried out</t>
+  </si>
+  <si>
+    <t>modified</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>A rule describing a recommendation for performing an activity</t>
+  </si>
+  <si>
+    <t>Recommendations are aligned with the term SHOULD in RFC2119 where specified activities should be carried out but are not obligations</t>
+  </si>
+  <si>
+    <t>Obligation</t>
+  </si>
+  <si>
+    <t>A rule describing an obligation for performing an activity</t>
+  </si>
+  <si>
+    <t>Obligations are aligned with the term MUST in RFC2119 where specified activities are mandatory to be carried out</t>
+  </si>
+  <si>
+    <t>UnacceptableRule</t>
+  </si>
+  <si>
+    <t>Unacceptable Rule</t>
+  </si>
+  <si>
+    <t>A rule that is unacceptable where it not desirable if it occurs</t>
+  </si>
+  <si>
+    <t>Unacceptable is a subjective concept that enables specifying something is to be avoided as compared to "acceptable". By itself it does not signal any deterrence or prohibition - for which further specific concepts are defined</t>
+  </si>
+  <si>
+    <t>Deterrence</t>
+  </si>
+  <si>
+    <t>A rule describing a deterrence for performing an activity</t>
+  </si>
+  <si>
+    <t>dpv:UnacceptableRule</t>
+  </si>
+  <si>
+    <t>Deterrences are aligned with the term SHOULD NOT in RFC2119 where specified activities should be avoided from being carried out but are not prohibitions</t>
   </si>
   <si>
     <t>Prohibition</t>
@@ -92,10 +158,7 @@
     <t>A rule describing a prohibition to perform an activity</t>
   </si>
   <si>
-    <t>Obligation</t>
-  </si>
-  <si>
-    <t>A rule describing an obligation for performing an activity</t>
+    <t>Prohibitions are aligned with the term MUST NOT in RFC2119 where specified activities are prohibited from being carried out</t>
   </si>
   <si>
     <t>RuleFulfilmentStatus</t>
@@ -218,6 +281,42 @@
     <t>Status indicating a permission has not been utilised i.e. the activity stated as being permitted has not been carried out</t>
   </si>
   <si>
+    <t>RecommendationUtilised</t>
+  </si>
+  <si>
+    <t>Recommendation Utilised</t>
+  </si>
+  <si>
+    <t>Status indicating a recommendation has been utilised i.e. the activity stated as being recommended has been carried out</t>
+  </si>
+  <si>
+    <t>RecommendationNotUtilised</t>
+  </si>
+  <si>
+    <t>Recommendation Not Utilised</t>
+  </si>
+  <si>
+    <t>Status indicating a recommendation has not been utilised i.e. the activity stated as being recommended has not been carried out</t>
+  </si>
+  <si>
+    <t>DeterrenceUtilised</t>
+  </si>
+  <si>
+    <t>Deterrence Utilised</t>
+  </si>
+  <si>
+    <t>Status indicating a deterrence has been utilised i.e. the activity stated as being deterred has not been carried out</t>
+  </si>
+  <si>
+    <t>DeterrenceNotUtilised</t>
+  </si>
+  <si>
+    <t>Deterrence Not Utilised</t>
+  </si>
+  <si>
+    <t>Status indicating a deterrence has not been utilised i.e. the activity stated as being deterred has been carried out</t>
+  </si>
+  <si>
     <t>domain</t>
   </si>
   <si>
@@ -233,7 +332,7 @@
     <t>has rule</t>
   </si>
   <si>
-    <t>Specifying applicability or inclusion of a rule within specified context</t>
+    <t>Specifies applicability or inclusion of a rule within specified context</t>
   </si>
   <si>
     <t>dpv:Context</t>
@@ -248,7 +347,7 @@
     <t>has permission</t>
   </si>
   <si>
-    <t>Specifying applicability or inclusion of a permission rule within specified context</t>
+    <t>Specifies applicability or inclusion of a permission rule within specified context</t>
   </si>
   <si>
     <t>dpv:Permission</t>
@@ -257,37 +356,61 @@
     <t>dpv:hasRule</t>
   </si>
   <si>
+    <t>hasRecommendation</t>
+  </si>
+  <si>
+    <t>has recommendation</t>
+  </si>
+  <si>
+    <t>Specifies applicability or inclusion of a recommendation rule within specified context</t>
+  </si>
+  <si>
+    <t>dpv:Recommendation</t>
+  </si>
+  <si>
+    <t>hasObligation</t>
+  </si>
+  <si>
+    <t>has obligation</t>
+  </si>
+  <si>
+    <t>Specifies applicability or inclusion of an obligation rule within specified context</t>
+  </si>
+  <si>
+    <t>dpv:Obligation</t>
+  </si>
+  <si>
+    <t>hasDeterrence</t>
+  </si>
+  <si>
+    <t>has deterrence</t>
+  </si>
+  <si>
+    <t>Specifies applicability or inclusion of a deterrence rule within specified context</t>
+  </si>
+  <si>
+    <t>dpv:Deterrence</t>
+  </si>
+  <si>
     <t>hasProhibition</t>
   </si>
   <si>
     <t>has prohibition</t>
   </si>
   <si>
-    <t>Specifying applicability or inclusion of a prohibition rule within specified context</t>
+    <t>Specifies applicability or inclusion of a prohibition rule within specified context</t>
   </si>
   <si>
     <t>dpv:Prohibition</t>
   </si>
   <si>
-    <t>hasObligation</t>
-  </si>
-  <si>
-    <t>has obligation</t>
-  </si>
-  <si>
-    <t>Specifying applicability or inclusion of an obligation rule within specified context</t>
-  </si>
-  <si>
-    <t>dpv:Obligation</t>
-  </si>
-  <si>
-    <t>hasFulfillmentsStatus</t>
-  </si>
-  <si>
-    <t>has fulfillment status</t>
-  </si>
-  <si>
-    <t>Specifying the fulfillment status associated with a rule</t>
+    <t>hasFulfilmentStatus</t>
+  </si>
+  <si>
+    <t>has fulfilment status</t>
+  </si>
+  <si>
+    <t>Specifies the fulfillment status associated with a rule</t>
   </si>
   <si>
     <t>dpv:hasStatus</t>
@@ -324,13 +447,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF274E13"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -454,10 +577,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -474,7 +597,7 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -884,81 +1007,44 @@
       <c r="AF2" s="11"/>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12">
-        <v>44853.0</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="11"/>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="K3" s="12"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="11"/>
       <c r="K4" s="12">
-        <v>44853.0</v>
-      </c>
-      <c r="L4" s="12"/>
+        <v>45827.0</v>
+      </c>
+      <c r="L4" s="11"/>
       <c r="M4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
@@ -981,32 +1067,38 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="11"/>
+        <v>28</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="E5" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="J5" s="11"/>
       <c r="K5" s="12">
         <v>44853.0</v>
       </c>
-      <c r="L5" s="11"/>
+      <c r="L5" s="12">
+        <v>45827.0</v>
+      </c>
       <c r="M5" s="10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
@@ -1028,41 +1120,91 @@
       <c r="AF5" s="11"/>
     </row>
     <row r="6">
-      <c r="B6" s="14"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="12"/>
+      <c r="A6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="12">
+        <v>45827.0</v>
+      </c>
       <c r="L6" s="12"/>
+      <c r="M6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="13"/>
+      <c r="I7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="11"/>
       <c r="K7" s="12">
-        <v>45545.0</v>
-      </c>
-      <c r="L7" s="12"/>
+        <v>44853.0</v>
+      </c>
+      <c r="L7" s="12">
+        <v>45827.0</v>
+      </c>
       <c r="M7" s="10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
@@ -1083,54 +1225,6 @@
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
     </row>
-    <row r="8">
-      <c r="A8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="12">
-        <v>45545.0</v>
-      </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-    </row>
     <row r="9">
       <c r="A9" s="10" t="s">
         <v>38</v>
@@ -1143,22 +1237,24 @@
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="I9" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="J9" s="11"/>
       <c r="K9" s="12">
-        <v>45545.0</v>
+        <v>45827.0</v>
       </c>
       <c r="L9" s="11"/>
       <c r="M9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
@@ -1181,7 +1277,7 @@
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>42</v>
@@ -1189,24 +1285,28 @@
       <c r="C10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="E10" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="I10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J10" s="14"/>
       <c r="K10" s="12">
-        <v>45545.0</v>
-      </c>
-      <c r="L10" s="11"/>
+        <v>45827.0</v>
+      </c>
+      <c r="L10" s="12"/>
       <c r="M10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
@@ -1229,36 +1329,40 @@
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="14"/>
       <c r="K11" s="12">
-        <v>45545.0</v>
-      </c>
-      <c r="L11" s="12"/>
+        <v>44853.0</v>
+      </c>
+      <c r="L11" s="12">
+        <v>45827.0</v>
+      </c>
       <c r="M11" s="10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O11" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="O11" s="11"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
@@ -1278,85 +1382,41 @@
       <c r="AF11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="12">
-        <v>45545.0</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
+      <c r="B12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="12">
         <v>45545.0</v>
       </c>
-      <c r="L13" s="11"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -1387,17 +1447,15 @@
       <c r="C14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="12">
         <v>45545.0</v>
       </c>
@@ -1406,7 +1464,7 @@
         <v>19</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
@@ -1437,26 +1495,24 @@
       <c r="C15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="18"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
       <c r="K15" s="12">
         <v>45545.0</v>
       </c>
-      <c r="L15" s="12"/>
+      <c r="L15" s="11"/>
       <c r="M15" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
@@ -1487,17 +1543,15 @@
       <c r="C16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11"/>
+      <c r="E16" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
-      <c r="J16" s="16"/>
+      <c r="J16" s="11"/>
       <c r="K16" s="12">
         <v>45545.0</v>
       </c>
@@ -1506,7 +1560,7 @@
         <v>19</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
@@ -1534,31 +1588,31 @@
       <c r="B17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="15" t="s">
         <v>67</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>37</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="J17" s="16"/>
       <c r="K17" s="12">
         <v>45545.0</v>
       </c>
-      <c r="L17" s="11"/>
+      <c r="L17" s="12"/>
       <c r="M17" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="11"/>
+        <v>54</v>
+      </c>
+      <c r="O17" s="17"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
@@ -1578,34 +1632,504 @@
       <c r="AF17" s="11"/>
     </row>
     <row r="18">
-      <c r="B18" s="20"/>
+      <c r="A18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="11"/>
     </row>
     <row r="19">
-      <c r="B19" s="20"/>
+      <c r="A19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
     </row>
     <row r="20">
-      <c r="B20" s="20"/>
+      <c r="A20" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+      <c r="AA20" s="11"/>
+      <c r="AB20" s="11"/>
+      <c r="AC20" s="11"/>
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="11"/>
+      <c r="AF20" s="11"/>
     </row>
     <row r="21">
-      <c r="B21" s="20"/>
+      <c r="A21" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L21" s="12"/>
+      <c r="M21" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="11"/>
+      <c r="Y21" s="11"/>
+      <c r="Z21" s="11"/>
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="11"/>
+      <c r="AC21" s="11"/>
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="11"/>
+      <c r="AF21" s="11"/>
     </row>
     <row r="22">
-      <c r="B22" s="20"/>
+      <c r="A22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="11"/>
+      <c r="AF22" s="11"/>
     </row>
     <row r="23">
-      <c r="B23" s="20"/>
+      <c r="A23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
     </row>
     <row r="24">
-      <c r="B24" s="20"/>
+      <c r="A24" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="12">
+        <v>45827.0</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
+      <c r="Z24" s="11"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="11"/>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="11"/>
     </row>
     <row r="25">
-      <c r="B25" s="20"/>
+      <c r="A25" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="12">
+        <v>45827.0</v>
+      </c>
+      <c r="L25" s="11"/>
+      <c r="M25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="11"/>
     </row>
     <row r="26">
-      <c r="B26" s="20"/>
+      <c r="A26" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="12">
+        <v>45827.0</v>
+      </c>
+      <c r="L26" s="11"/>
+      <c r="M26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="11"/>
+      <c r="AF26" s="11"/>
     </row>
     <row r="27">
-      <c r="B27" s="20"/>
+      <c r="A27" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="12">
+        <v>45827.0</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="11"/>
+      <c r="AC27" s="11"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="11"/>
+      <c r="AF27" s="11"/>
     </row>
     <row r="28">
       <c r="B28" s="20"/>
@@ -4178,28 +4702,43 @@
     <row r="884">
       <c r="B884" s="20"/>
     </row>
+    <row r="885">
+      <c r="B885" s="20"/>
+    </row>
+    <row r="886">
+      <c r="B886" s="20"/>
+    </row>
+    <row r="887">
+      <c r="B887" s="20"/>
+    </row>
+    <row r="888">
+      <c r="B888" s="20"/>
+    </row>
+    <row r="889">
+      <c r="B889" s="20"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:J2 K2:K5 L2:M2 N2:N6 O2:AF2">
+  <conditionalFormatting sqref="A2:J2 K2:K11 L2:M2 N2:N12 O2:AF2 N24:N27">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J2 K2:K5 L2:M2 N2:N6 O2:AF2">
+  <conditionalFormatting sqref="A2:J2 K2:K11 L2:M2 N2:N12 O2:AF2 N24:N27">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF834">
+  <conditionalFormatting sqref="A2:AF839">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF834">
+  <conditionalFormatting sqref="A2:AF839">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF834">
+  <conditionalFormatting sqref="A2:AF839">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>$M2="modified"</formula>
     </cfRule>
@@ -4247,13 +4786,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -4285,22 +4824,22 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>72</v>
+        <v>104</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -4333,22 +4872,22 @@
     </row>
     <row r="3">
       <c r="A3" s="10" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -4381,36 +4920,36 @@
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="12">
-        <v>44853.0</v>
+        <v>45827.0</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
@@ -4429,22 +4968,22 @@
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -4477,36 +5016,36 @@
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>91</v>
+        <v>123</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>23</v>
+        <v>125</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="12">
-        <v>45545.0</v>
+        <v>45827.0</v>
       </c>
       <c r="L6" s="11"/>
       <c r="M6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -4524,10 +5063,84 @@
       <c r="AB6" s="11"/>
     </row>
     <row r="7">
-      <c r="C7" s="23"/>
+      <c r="A7" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="12">
+        <v>44853.0</v>
+      </c>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
     </row>
     <row r="8">
-      <c r="C8" s="23"/>
+      <c r="A8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="12">
+        <v>45545.0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>45827.0</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9">
       <c r="C9" s="23"/>
@@ -7451,28 +8064,34 @@
     <row r="982">
       <c r="C982" s="23"/>
     </row>
+    <row r="983">
+      <c r="C983" s="23"/>
+    </row>
+    <row r="984">
+      <c r="C984" s="23"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K5">
+  <conditionalFormatting sqref="K2:K7 L8">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K5">
+  <conditionalFormatting sqref="K2:K7 L8">
     <cfRule type="expression" dxfId="4" priority="2">
       <formula>$M2="modified"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB300">
+  <conditionalFormatting sqref="A2:AB302">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB200">
+  <conditionalFormatting sqref="A2:AB202">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B3 C2:D17 E2:E3 F2:F17 G2:J3 K2:K17 L2:AB3 A6:B17 E6:E17 G6:J17 L6:AB17">
+  <conditionalFormatting sqref="A2:B3 C2:D19 E2:E3 F2:F19 G2:J3 K2:K19 L2:AB3 A8:B19 E8:E19 G8:J19 L8:AB19">
     <cfRule type="expression" dxfId="1" priority="5">
       <formula>$M2="deprecated"</formula>
     </cfRule>

</xml_diff>